<commit_message>
pretrain mobileNetV2 with new image and data auguments
</commit_message>
<xml_diff>
--- a/Chapter04-Convolutional-Neural-Networks/DeepConvolutional_Models-CaseStudies/cases studies.xlsx
+++ b/Chapter04-Convolutional-Neural-Networks/DeepConvolutional_Models-CaseStudies/cases studies.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AI-learning\Deep-learning\Chapter04-Convolutional-Neural-Networks\DeepConvolutional_Models-CaseStudies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FF426F9-837E-4E81-8528-67C36F046CCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE4733A8-90F5-4E07-952E-EF6A03A7ABBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-15870" windowWidth="25440" windowHeight="15270" activeTab="1" xr2:uid="{CCDBED70-31EF-43E7-BAA9-99EBC844BBE9}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" activeTab="1" xr2:uid="{CCDBED70-31EF-43E7-BAA9-99EBC844BBE9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -3195,10 +3195,10 @@
     <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1">
@@ -3257,8 +3257,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="14878050" y="1933575"/>
-          <a:ext cx="1000125" cy="1190625"/>
+          <a:off x="14868525" y="1885950"/>
+          <a:ext cx="1000125" cy="1162050"/>
           <a:chOff x="7620000" y="1695450"/>
           <a:chExt cx="1000125" cy="1190625"/>
         </a:xfrm>
@@ -3855,10 +3855,10 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>95252</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>114299</xdr:rowOff>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
@@ -3879,8 +3879,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="2314577" y="1476374"/>
-          <a:ext cx="3457574" cy="1876425"/>
+          <a:off x="3400425" y="1414463"/>
+          <a:ext cx="2366964" cy="1852611"/>
           <a:chOff x="7620000" y="1681802"/>
           <a:chExt cx="986023" cy="1204273"/>
         </a:xfrm>
@@ -5747,8 +5747,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A62F38A1-C4AC-4BD3-899D-DDDC5242902E}">
   <dimension ref="C3:Z63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="X25" sqref="X25"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="F68" sqref="F68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>

</xml_diff>